<commit_message>
Update 11-1-2024 Transfer Task Done
</commit_message>
<xml_diff>
--- a/UploadedFiles/transfer.xlsx
+++ b/UploadedFiles/transfer.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kirolos\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kirolos\Desktop\Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56027E9C-914E-4D4B-9006-159D84071C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3C34F7-49B0-4D73-9A9D-75A0B54E9650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{05031A61-708A-4E91-B92C-51AFD033B701}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,9 +34,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>IMEI</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>DeviceType</t>
   </si>
 </sst>
 </file>
@@ -80,13 +92,15 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,41 +414,102 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF2C4E7-C919-4E96-8556-BF79D08C6945}">
-  <dimension ref="A1:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01872A20-942F-41A8-926E-C5A556EAF55B}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="16.125" customWidth="1"/>
+    <col min="2" max="2" width="13.125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>354505555602861</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>352019334695651</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>45352</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>354505555605146</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>352019334695677</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>45352</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>354505555605260</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>352019334695693</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>45352</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>354505555605328</v>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>352019334695719</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>45352</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>352019334695735</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>45352</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>